<commit_message>
Included Supplier and Store cadastres
</commit_message>
<xml_diff>
--- a/PortalDoFranqueado.Export/Resources/PurchaseModel.xlsx
+++ b/PortalDoFranqueado.Export/Resources/PurchaseModel.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$9:$Q$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$9:$R$9</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Pedido do Franqueado</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Qtd</t>
+  </si>
+  <si>
+    <t>&lt;CNPJ&gt;</t>
+  </si>
+  <si>
+    <t>Fornecedor</t>
+  </si>
+  <si>
+    <t>&lt;Fornecedor&gt;</t>
   </si>
 </sst>
 </file>
@@ -224,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,6 +280,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -278,11 +290,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -590,83 +603,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
-    <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" customWidth="1"/>
-    <col min="10" max="10" width="6" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" customWidth="1"/>
-    <col min="12" max="12" width="6" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" customWidth="1"/>
-    <col min="14" max="14" width="6" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" customWidth="1"/>
-    <col min="16" max="16" width="6" customWidth="1"/>
-    <col min="17" max="17" width="8.28515625" customWidth="1"/>
-    <col min="18" max="19" width="13.28515625" customWidth="1"/>
+    <col min="2" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="6" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" customWidth="1"/>
+    <col min="13" max="13" width="6" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" customWidth="1"/>
+    <col min="15" max="15" width="6" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" customWidth="1"/>
+    <col min="17" max="17" width="6" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" customWidth="1"/>
+    <col min="19" max="20" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-    </row>
-    <row r="2" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+    </row>
+    <row r="2" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="6"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D3" s="2"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="6"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -680,13 +696,13 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="21"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -694,64 +710,69 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C5" s="5"/>
+      <c r="H5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C6" s="16"/>
+      <c r="H6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="17"/>
-      <c r="G7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C7" s="17"/>
+      <c r="H7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="17"/>
-      <c r="G8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C8" s="17"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>2</v>
       </c>
@@ -759,119 +780,126 @@
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="N9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="O9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="7" t="s">
+      <c r="P9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="Q9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="R9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R9" s="8" t="s">
+      <c r="S9" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="20"/>
+      <c r="F10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="20"/>
+      <c r="H10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="20"/>
+      <c r="L10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="20"/>
+      <c r="N10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="23"/>
-      <c r="O10" s="19" t="s">
+      <c r="O10" s="20"/>
+      <c r="P10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="19" t="s">
+      <c r="Q10" s="20"/>
+      <c r="R10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="R10" s="18" t="e">
-        <f>SUM(E10,G10,I10,K10,M10,O10,Q10)*C10</f>
+      <c r="S10" s="18" t="e">
+        <f>SUM(F10,H10,J10,L10,N10,P10,R10)*D10</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="12"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="12"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="10"/>
+      <c r="R11" s="1"/>
       <c r="S11" s="10"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="10"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -891,8 +919,9 @@
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="10"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -912,12 +941,13 @@
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="10"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -931,31 +961,33 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="13"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R14" s="2"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="13"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="12"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="12"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="10"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R15" s="1"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="10"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -973,10 +1005,11 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="10"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R16" s="10"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="10"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -996,8 +1029,9 @@
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="10"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -1017,8 +1051,9 @@
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -1038,8 +1073,9 @@
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -1057,15 +1093,17 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:Q9"/>
-  <mergeCells count="3">
+  <autoFilter ref="A9:R9"/>
+  <mergeCells count="4">
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="B2:O2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>